<commit_message>
add api + test api
</commit_message>
<xml_diff>
--- a/db/users.xlsx
+++ b/db/users.xlsx
@@ -97,7 +97,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -135,10 +135,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,7 +454,7 @@
     <col min="4" max="4" style="3" width="24.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -482,7 +482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -494,7 +494,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -508,7 +508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -522,7 +522,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -536,7 +536,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>